<commit_message>
fix on oc service
</commit_message>
<xml_diff>
--- a/documentation/LagIncreaseDo.xlsx
+++ b/documentation/LagIncreaseDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiamarilli/Progetti/unifi_phd/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69A10FF-420E-AA4A-AC0B-559268664FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E39147-14A6-0E46-88D3-912F62EF07CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" activeTab="1" xr2:uid="{9C1D837C-A722-4248-A86A-CE69ED4B7649}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" activeTab="9" xr2:uid="{9C1D837C-A722-4248-A86A-CE69ED4B7649}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F16587F-151E-F944-A7AD-47F9A723EED8}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:K29"/>
     </sheetView>
   </sheetViews>
@@ -811,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE50FE21-6C3F-A64C-8473-A905EC1E2CAA}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:K29"/>
     </sheetView>
   </sheetViews>

</xml_diff>